<commit_message>
added the ability to sort people into categories based on event
</commit_message>
<xml_diff>
--- a/team_data/Scioly test data.xlsx
+++ b/team_data/Scioly test data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -118,7 +118,7 @@
     <t>goober, pete</t>
   </si>
   <si>
-    <t>Entomology, Experimental Design, material Science</t>
+    <t>Entomology, Experimental Design, Material Science</t>
   </si>
   <si>
     <t>Dynamic Planet</t>
@@ -142,7 +142,7 @@
     <t>roger, roy</t>
   </si>
   <si>
-    <t>Experimental design, Forensics</t>
+    <t>Experimental Design, Forensics</t>
   </si>
   <si>
     <t>Geologic Mapping</t>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>Write It Do It</t>
+  </si>
+  <si>
+    <t>Microbe Mission</t>
   </si>
 </sst>
 </file>
@@ -914,6 +917,11 @@
         <v>2.0</v>
       </c>
     </row>
+    <row r="24">
+      <c r="F24" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
the algorithm can now calculate the amount of teams needed
</commit_message>
<xml_diff>
--- a/team_data/Scioly test data.xlsx
+++ b/team_data/Scioly test data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -121,7 +121,7 @@
     <t>Entomology, Experimental Design, Material Science</t>
   </si>
   <si>
-    <t>Dynamic Planet</t>
+    <t>Optics</t>
   </si>
   <si>
     <t>pete</t>
@@ -130,7 +130,7 @@
     <t>idk, goober</t>
   </si>
   <si>
-    <t>Fossils, Material Science, Robot tour</t>
+    <t>Fossils, Material Science, Robot Tour</t>
   </si>
   <si>
     <t>Fossils</t>
@@ -163,7 +163,7 @@
     <t>roger, tom, Tim Tim</t>
   </si>
   <si>
-    <t>Experimental design, Optics</t>
+    <t>Experimental Design, Optics</t>
   </si>
   <si>
     <t>Forensics</t>
@@ -175,7 +175,7 @@
     <t>goober, pete, alex</t>
   </si>
   <si>
-    <t>Optics, Write it do it</t>
+    <t>Optics, Write It Do It</t>
   </si>
   <si>
     <t>Materials Science</t>
@@ -190,9 +190,6 @@
     <t>Anatomy and Physiology, Geologic Mapping</t>
   </si>
   <si>
-    <t>Optics</t>
-  </si>
-  <si>
     <t>bob</t>
   </si>
   <si>
@@ -211,7 +208,7 @@
     <t>johnny, javardo dominguez</t>
   </si>
   <si>
-    <t>Write it do it, Electric Vehicle</t>
+    <t>Write It Do It, Electric Vehicle</t>
   </si>
   <si>
     <t>Wind Power</t>
@@ -223,7 +220,7 @@
     <t>alex, goober</t>
   </si>
   <si>
-    <t>Electric Vehicle, Dynamic planet</t>
+    <t>Electric Vehicle, Dynamic Planet</t>
   </si>
   <si>
     <t>Electric Vehicle</t>
@@ -794,7 +791,7 @@
         <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="J13" s="1">
         <v>2.0</v>
@@ -802,19 +799,19 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J14" s="1">
         <v>2.0</v>
@@ -822,19 +819,19 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J15" s="1">
         <v>2.0</v>
@@ -842,19 +839,19 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J16" s="1">
         <v>2.0</v>
@@ -862,7 +859,7 @@
     </row>
     <row r="17">
       <c r="F17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J17" s="1">
         <v>2.0</v>
@@ -870,7 +867,7 @@
     </row>
     <row r="18">
       <c r="F18" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J18" s="1">
         <v>3.0</v>
@@ -878,7 +875,7 @@
     </row>
     <row r="19">
       <c r="F19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J19" s="1">
         <v>2.0</v>
@@ -886,7 +883,7 @@
     </row>
     <row r="20">
       <c r="F20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J20" s="1">
         <v>2.0</v>
@@ -894,7 +891,7 @@
     </row>
     <row r="21">
       <c r="F21" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1">
@@ -903,7 +900,7 @@
     </row>
     <row r="22">
       <c r="F22" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J22" s="1">
         <v>3.0</v>
@@ -911,7 +908,7 @@
     </row>
     <row r="23">
       <c r="F23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J23" s="1">
         <v>2.0</v>
@@ -919,7 +916,10 @@
     </row>
     <row r="24">
       <c r="F24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="J24" s="1">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>